<commit_message>
Отладил функции get_connection() и get_all_questions().
</commit_message>
<xml_diff>
--- a/app/database/questions_template.xlsx
+++ b/app/database/questions_template.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725CFF38-D383-B148-A3B9-1E5E38C33691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="page" sheetId="1" r:id="rId1"/>
@@ -114,7 +115,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -170,7 +171,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -450,20 +451,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="54.5" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -479,7 +480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -487,7 +488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -495,7 +496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -503,7 +504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -511,7 +512,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -519,7 +520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -527,7 +528,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -535,7 +536,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -543,7 +544,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -551,7 +552,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -559,7 +560,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -567,7 +568,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -575,13 +576,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1"/>
+  <autoFilter ref="A1:B1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Рефакторинг функций get_connection(), get_all_questions() и add_questions_from_excel().
</commit_message>
<xml_diff>
--- a/app/database/questions_template.xlsx
+++ b/app/database/questions_template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725CFF38-D383-B148-A3B9-1E5E38C33691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493362F3-D284-4F40-9010-94D889E07C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6480" yWindow="5140" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="page" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Вопрос</t>
   </si>
@@ -34,82 +34,19 @@
     <t>вопрос1</t>
   </si>
   <si>
-    <t>ответ1</t>
-  </si>
-  <si>
-    <t>вопрос2</t>
-  </si>
-  <si>
     <t>ответ2</t>
   </si>
   <si>
     <t>вопрос3</t>
   </si>
   <si>
-    <t>ответ3</t>
-  </si>
-  <si>
-    <t>вопрос4</t>
-  </si>
-  <si>
-    <t>ответ4</t>
-  </si>
-  <si>
-    <t>вопрос5</t>
-  </si>
-  <si>
-    <t>ответ5</t>
-  </si>
-  <si>
-    <t>вопрос6</t>
-  </si>
-  <si>
-    <t>ответ6</t>
-  </si>
-  <si>
-    <t>вопрос7</t>
-  </si>
-  <si>
-    <t>ответ7</t>
-  </si>
-  <si>
-    <t>вопрос8</t>
-  </si>
-  <si>
-    <t>ответ8</t>
-  </si>
-  <si>
-    <t>вопрос9</t>
-  </si>
-  <si>
-    <t>ответ9</t>
-  </si>
-  <si>
-    <t>вопрос10</t>
-  </si>
-  <si>
-    <t>ответ10</t>
-  </si>
-  <si>
-    <t>вопрос11</t>
-  </si>
-  <si>
-    <t>ответ11</t>
-  </si>
-  <si>
-    <t>вопрос12</t>
-  </si>
-  <si>
-    <t>ответ12</t>
-  </si>
-  <si>
-    <t>вопрос13</t>
-  </si>
-  <si>
-    <t>ответ13</t>
-  </si>
-  <si>
-    <t>вопрос14</t>
+    <t>вопрос 4</t>
+  </si>
+  <si>
+    <t>ответ 4</t>
+  </si>
+  <si>
+    <t>ответ25</t>
   </si>
 </sst>
 </file>
@@ -452,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -477,108 +414,25 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>